<commit_message>
JLCpcb production files ready
</commit_message>
<xml_diff>
--- a/kicad/gerber/veloce-top-pos.xlsx
+++ b/kicad/gerber/veloce-top-pos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t xml:space="preserve">R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29</t>
   </si>
 </sst>
 </file>
@@ -233,10 +272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="A:E"/>
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -267,10 +306,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>-68</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -284,10 +323,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>-78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -301,10 +340,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>-88</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -318,10 +357,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>-98</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -335,10 +374,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>-108</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -352,10 +391,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>-118</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -369,10 +408,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>-128</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
@@ -386,10 +425,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>-138</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -403,10 +442,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>163.5</v>
+        <v>22.5</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>-68</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -420,10 +459,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>163.5</v>
+        <v>22.5</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>-78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>6</v>
@@ -437,10 +476,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>160.5</v>
+        <v>19.5</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>-88</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
@@ -454,10 +493,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>160.5</v>
+        <v>19.5</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>-98</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -471,10 +510,10 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>160.5</v>
+        <v>19.5</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>-108</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -488,10 +527,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>160.5</v>
+        <v>19.5</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>-118</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -505,10 +544,10 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>160.5</v>
+        <v>19.5</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>-128</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -522,10 +561,10 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>160.5</v>
+        <v>19.5</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>-138</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
@@ -539,10 +578,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>172.5</v>
+        <v>31.5</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>-70.5</v>
+        <v>84.5</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -556,10 +595,10 @@
         <v>23</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>172.5</v>
+        <v>31.5</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>-80.5</v>
+        <v>74.5</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
@@ -573,16 +612,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>172.5</v>
+        <v>31.5</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>-65.5</v>
+        <v>89.5</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,16 +629,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>172.5</v>
+        <v>31.5</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>-75.5</v>
+        <v>79.5</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,10 +646,10 @@
         <v>26</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>-89</v>
+        <v>66</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
@@ -624,10 +663,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>-99</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>6</v>
@@ -641,16 +680,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>-87</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,16 +697,16 @@
         <v>29</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>-97</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,10 +714,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>-109</v>
+        <v>46</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
@@ -692,10 +731,10 @@
         <v>31</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>-119</v>
+        <v>36</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
@@ -709,16 +748,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>-107</v>
+        <v>48</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,16 +765,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>-117</v>
+        <v>38</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,10 +782,10 @@
         <v>34</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>-129</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>6</v>
@@ -760,10 +799,10 @@
         <v>35</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>-139</v>
+        <v>16</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
@@ -777,16 +816,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>-127</v>
+        <v>28</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,16 +833,237 @@
         <v>37</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>164.5</v>
+        <v>23.5</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>-137</v>
+        <v>18</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>59.29</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>59.29</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>70.29</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>70.29</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>69.5</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>59.5</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>83.81</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>